<commit_message>
Updated all dice boards with smaller programming connector. Added ChargerV16
</commit_message>
<xml_diff>
--- a/Dice/D10/D10v2/D10V2 BOM.xlsx
+++ b/Dice/D10/D10v2/D10V2 BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Pixels-dice\Electrical\Dice\D10\D10v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6D0A847-9C2E-4C89-9D4E-1DF1DD170147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5AB44A9E-77F6-46F7-B5C9-7E74113B50AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14430" yWindow="990" windowWidth="29250" windowHeight="19875"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="34425" windowHeight="20160"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="172">
   <si>
     <t>Source:</t>
   </si>
@@ -55,6 +55,9 @@
     <t>Manufacturer Part Number</t>
   </si>
   <si>
+    <t>Pixels Part Number</t>
+  </si>
+  <si>
     <t>AE1</t>
   </si>
   <si>
@@ -91,6 +94,9 @@
     <t>GRM155R61A475MEAAJ</t>
   </si>
   <si>
+    <t>SMD-C002</t>
+  </si>
+  <si>
     <t>C2, C5</t>
   </si>
   <si>
@@ -100,6 +106,9 @@
     <t>GRT1555C2A8R0DA02</t>
   </si>
   <si>
+    <t>SMD-C001</t>
+  </si>
+  <si>
     <t>C3, C10, C23, C24</t>
   </si>
   <si>
@@ -109,6 +118,9 @@
     <t>GRM155R61H104KE19D</t>
   </si>
   <si>
+    <t>SMD-C005</t>
+  </si>
+  <si>
     <t>C7</t>
   </si>
   <si>
@@ -118,6 +130,9 @@
     <t>GCM1555C1H101JA16J</t>
   </si>
   <si>
+    <t>SMD-C003</t>
+  </si>
+  <si>
     <t>C8</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
     <t>GJM1555C1HR80BB01</t>
   </si>
   <si>
+    <t>SMD-C004</t>
+  </si>
+  <si>
     <t>C9, C16</t>
   </si>
   <si>
@@ -160,6 +178,9 @@
     <t>GRM188R61E475KE11D</t>
   </si>
   <si>
+    <t>SMD-C010</t>
+  </si>
+  <si>
     <t>C15</t>
   </si>
   <si>
@@ -181,6 +202,9 @@
     <t>GRM3195C1H333JA01J</t>
   </si>
   <si>
+    <t>SMD-C011</t>
+  </si>
+  <si>
     <t>C21, C22</t>
   </si>
   <si>
@@ -190,6 +214,9 @@
     <t>GRM155R71H103KA88</t>
   </si>
   <si>
+    <t>SMD-C009</t>
+  </si>
+  <si>
     <t>D1</t>
   </si>
   <si>
@@ -205,6 +232,9 @@
     <t>BAV99S,115</t>
   </si>
   <si>
+    <t>SMD-D001</t>
+  </si>
+  <si>
     <t>D2, D3, D4, D5, D6, D7, D8, D9, D10, D11</t>
   </si>
   <si>
@@ -220,6 +250,9 @@
     <t>TX1812Z 2020</t>
   </si>
   <si>
+    <t>SMD-D002-ALT2</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -232,6 +265,9 @@
     <t>LQM21FN100M80L</t>
   </si>
   <si>
+    <t>SMD-L001</t>
+  </si>
+  <si>
     <t>L2</t>
   </si>
   <si>
@@ -244,6 +280,9 @@
     <t>LQG15HS15NJ02D</t>
   </si>
   <si>
+    <t>SMD-L002</t>
+  </si>
+  <si>
     <t>L3</t>
   </si>
   <si>
@@ -277,6 +316,9 @@
     <t>0402WGF4024TCE</t>
   </si>
   <si>
+    <t>SMD-R003</t>
+  </si>
+  <si>
     <t>R3</t>
   </si>
   <si>
@@ -286,6 +328,9 @@
     <t>0402WGJ0103TCE</t>
   </si>
   <si>
+    <t>SMD-R002</t>
+  </si>
+  <si>
     <t>R4, R5</t>
   </si>
   <si>
@@ -298,6 +343,9 @@
     <t>0402WGF1003TCE</t>
   </si>
   <si>
+    <t>SMD-R006</t>
+  </si>
+  <si>
     <t>R6</t>
   </si>
   <si>
@@ -316,6 +364,9 @@
     <t>0402WGF1005TCE</t>
   </si>
   <si>
+    <t>SMD-R004</t>
+  </si>
+  <si>
     <t>R9</t>
   </si>
   <si>
@@ -337,6 +388,9 @@
     <t>0402WGJ0272TCE</t>
   </si>
   <si>
+    <t>SMD-R021</t>
+  </si>
+  <si>
     <t>TH1</t>
   </si>
   <si>
@@ -364,6 +418,9 @@
     <t>NRF52810-QCAA-R</t>
   </si>
   <si>
+    <t>SMD-U001</t>
+  </si>
+  <si>
     <t>U2</t>
   </si>
   <si>
@@ -376,6 +433,9 @@
     <t>Kionix</t>
   </si>
   <si>
+    <t>SMD-U002-ALT1</t>
+  </si>
+  <si>
     <t>U3</t>
   </si>
   <si>
@@ -415,6 +475,9 @@
     <t>Microchip</t>
   </si>
   <si>
+    <t>SMD-U005</t>
+  </si>
+  <si>
     <t>U6</t>
   </si>
   <si>
@@ -424,6 +487,9 @@
     <t>XI'AN Aerosemi Tech</t>
   </si>
   <si>
+    <t>SMD-U006-ALT2</t>
+  </si>
+  <si>
     <t>U7</t>
   </si>
   <si>
@@ -439,6 +505,9 @@
     <t>SN74LVC1G08DCKR</t>
   </si>
   <si>
+    <t>SMD-U007</t>
+  </si>
+  <si>
     <t>U8</t>
   </si>
   <si>
@@ -451,6 +520,9 @@
     <t>TMR1366S</t>
   </si>
   <si>
+    <t>SMD-U008-ALT8</t>
+  </si>
+  <si>
     <t>Y1</t>
   </si>
   <si>
@@ -461,6 +533,9 @@
   </si>
   <si>
     <t>XRCGB32M000F2P00R0</t>
+  </si>
+  <si>
+    <t>SMD-Y001</t>
   </si>
 </sst>
 </file>
@@ -784,7 +859,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -899,15 +974,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -953,16 +1019,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1318,24 +1377,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I60" sqref="I60"/>
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="31.5703125" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1343,974 +1393,1067 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>44928.526041666664</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+        <v>44960.60601851852</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>11</v>
+      <c r="C5" t="s">
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>17</v>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>23</v>
+      <c r="C7" t="s">
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
+      <c r="C8" t="s">
+        <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
+      <c r="C9" t="s">
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
+      <c r="C10" t="s">
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E10" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="I10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
+      <c r="C11" t="s">
+        <v>42</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
         <v>39</v>
       </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
+      <c r="C13" t="s">
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="I13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>46</v>
+      <c r="C14" t="s">
+        <v>53</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="I14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
       <c r="B15">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>49</v>
+      <c r="C15" t="s">
+        <v>56</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="I15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>53</v>
+      <c r="C16" t="s">
+        <v>61</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F16" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="I16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>56</v>
+      <c r="C17" t="s">
+        <v>65</v>
       </c>
       <c r="D17" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G17" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="H17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="I17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
       <c r="B18">
         <v>10</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>61</v>
+      <c r="C18" t="s">
+        <v>71</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="F18" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="H18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="I18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>66</v>
+      <c r="C19" t="s">
+        <v>77</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="I19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>70</v>
+      <c r="C20" t="s">
+        <v>82</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="E20" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F20" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="I20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>74</v>
+      <c r="C21" t="s">
+        <v>87</v>
       </c>
       <c r="D21" t="s">
-        <v>75</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F21" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>77</v>
+      <c r="C22" t="s">
+        <v>90</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G22" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>24</v>
       </c>
       <c r="B23">
         <v>3</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>80</v>
+      <c r="C23" t="s">
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="E23" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F23" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="I23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>25</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>85</v>
+      <c r="C24" t="s">
+        <v>99</v>
       </c>
       <c r="D24" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="E24" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G24" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="I24" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>26</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>88</v>
+      <c r="C25" t="s">
+        <v>103</v>
       </c>
       <c r="D25" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H25" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="I25" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>27</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>92</v>
+      <c r="C26" t="s">
+        <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="E26" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G26" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H26" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="I26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>28</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" t="s">
+        <v>111</v>
+      </c>
+      <c r="D27" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" t="s">
         <v>95</v>
       </c>
-      <c r="D27" t="s">
+      <c r="F27" t="s">
+        <v>21</v>
+      </c>
+      <c r="G27" t="s">
         <v>96</v>
       </c>
-      <c r="E27" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" t="s">
-        <v>20</v>
-      </c>
-      <c r="G27" t="s">
-        <v>83</v>
-      </c>
       <c r="H27" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I27" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>29</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>98</v>
+      <c r="C28" t="s">
+        <v>115</v>
       </c>
       <c r="D28" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G28" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H28" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="I28" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>30</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>101</v>
+      <c r="C29" t="s">
+        <v>118</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E29" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G29" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H29" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="I29" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>31</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>102</v>
+      <c r="C30" t="s">
+        <v>119</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="E30" t="s">
-        <v>82</v>
+        <v>95</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G30" t="s">
-        <v>83</v>
+        <v>96</v>
       </c>
       <c r="H30" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="I30" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>32</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" t="s">
+        <v>123</v>
+      </c>
+      <c r="D31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" t="s">
         <v>105</v>
       </c>
-      <c r="D31" t="s">
-        <v>106</v>
-      </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
       <c r="F31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="H31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>33</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>109</v>
+      <c r="C32" t="s">
+        <v>127</v>
       </c>
       <c r="D32" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
       <c r="F32" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="H32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="I32" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>34</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>114</v>
+      <c r="C33" t="s">
+        <v>133</v>
       </c>
       <c r="D33" t="s">
-        <v>115</v>
+        <v>134</v>
       </c>
       <c r="E33" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="F33" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G33" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="H33" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="I33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>35</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>118</v>
+      <c r="C34" t="s">
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F34" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G34" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="H34" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>36</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>122</v>
+      <c r="C35" t="s">
+        <v>142</v>
       </c>
       <c r="D35" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="E35" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G35" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="H35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>37</v>
       </c>
       <c r="B36">
         <v>1</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>127</v>
+      <c r="C36" t="s">
+        <v>147</v>
       </c>
       <c r="D36" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="E36" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="F36" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G36" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="H36" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="I36" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>38</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>131</v>
+      <c r="C37" t="s">
+        <v>152</v>
       </c>
       <c r="D37" t="s">
-        <v>132</v>
+        <v>153</v>
       </c>
       <c r="E37" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="F37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G37" t="s">
-        <v>133</v>
+        <v>154</v>
       </c>
       <c r="H37" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="I37" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>39</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>134</v>
+      <c r="C38" t="s">
+        <v>156</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>157</v>
       </c>
       <c r="E38" t="s">
-        <v>136</v>
+        <v>158</v>
       </c>
       <c r="F38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G38" t="s">
-        <v>137</v>
+        <v>159</v>
       </c>
       <c r="H38" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="I38" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>40</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>139</v>
+      <c r="C39" t="s">
+        <v>162</v>
       </c>
       <c r="D39" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" t="s">
         <v>140</v>
       </c>
-      <c r="E39" t="s">
-        <v>120</v>
-      </c>
       <c r="F39" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G39" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="H39" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="I39" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>59</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>143</v>
+      <c r="C40" t="s">
+        <v>167</v>
       </c>
       <c r="D40" t="s">
-        <v>144</v>
+        <v>168</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>169</v>
       </c>
       <c r="F40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G40" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H40" t="s">
-        <v>146</v>
+        <v>170</v>
+      </c>
+      <c r="I40" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>